<commit_message>
create contrasts for specific combintations of acqusitions
</commit_message>
<xml_diff>
--- a/fMRI/fx/SST/prepost_analysis/contrast_weights_stopsignal.xlsx
+++ b/fMRI/fx/SST/prepost_analysis/contrast_weights_stopsignal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristadestasio/Desktop/REV_scripts/fMRI/fx/SST/prepost_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC99118-DAFD-AC47-8054-1E486924EBB2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C4ABBD-B43C-A94F-84E7-9DED37B9D3A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16560" xr2:uid="{F44029D5-836C-9941-B0F2-754275B93E74}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16560" xr2:uid="{F44029D5-836C-9941-B0F2-754275B93E74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C102CF70-CBA0-A749-8140-E7CAFBFE284A}">
   <dimension ref="A1:XFD43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W12" workbookViewId="0">
-      <selection activeCell="AF33" sqref="AF33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43:AT43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
include motion columns in contrast weights
</commit_message>
<xml_diff>
--- a/fMRI/fx/SST/prepost_analysis/contrast_weights_stopsignal.xlsx
+++ b/fMRI/fx/SST/prepost_analysis/contrast_weights_stopsignal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristadestasio/Desktop/REV_scripts/fMRI/fx/SST/prepost_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C4ABBD-B43C-A94F-84E7-9DED37B9D3A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4F245D-3E89-3044-93C7-F2D92776CF6F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16560" xr2:uid="{F44029D5-836C-9941-B0F2-754275B93E74}"/>
   </bookViews>
@@ -600,7 +600,7 @@
   <dimension ref="A1:XFD43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43:AT43"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>